<commit_message>
Generate report Excel and config navigate details
</commit_message>
<xml_diff>
--- a/Optic.Api/wwwroot/template/Invoice.xlsx
+++ b/Optic.Api/wwwroot/template/Invoice.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\LAB\OPTICA\ARQUITECTURA\ARQUITECTURA 1\optic\Optic.Api\wwwroot\template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A237F8A-C46B-4C12-A4D4-B5EBF4077C05}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41B1F7E8-2AED-40F5-B9BD-207E6ADA54C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{7856CE4B-3B11-43C1-AC86-06E476F1C136}"/>
   </bookViews>
@@ -17,8 +17,7 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm.Print_Area" localSheetId="0">Formula!$A$1:$M$28</definedName>
-    <definedName name="Diagnosis">Formula!$E$14:$F$15</definedName>
-    <definedName name="Tags">Formula!$B$14:$D$15</definedName>
+    <definedName name="Details">Formula!$B$14:$H$15</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -41,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
   <si>
     <t>Nombre</t>
   </si>
@@ -50,12 +49,6 @@
   </si>
   <si>
     <t>Fecha</t>
-  </si>
-  <si>
-    <t>Tipo Lente:</t>
-  </si>
-  <si>
-    <t>Diagnostico:</t>
   </si>
   <si>
     <t>Observaciones</t>
@@ -65,28 +58,10 @@
 Teléfono: {{PhoneNumber}} - {{Address}} </t>
   </si>
   <si>
-    <t>{{item.Name}}</t>
-  </si>
-  <si>
-    <t>{{item.Value}}</t>
-  </si>
-  <si>
     <t>{{ClientName}}</t>
   </si>
   <si>
     <t>{{ClientPhoneNumber}}</t>
-  </si>
-  <si>
-    <t>{{FormulaDate}}</t>
-  </si>
-  <si>
-    <t>FORMULA #{{FormulaNumber}}</t>
-  </si>
-  <si>
-    <t>{{FormulaDescription}}</t>
-  </si>
-  <si>
-    <t>{{item}}</t>
   </si>
   <si>
     <t xml:space="preserve"> </t>
@@ -94,6 +69,42 @@
   <si>
     <t>Fecha de generación: {{GenerationDate}}
 Pasados 30 días no se responde por trabajos sin reclamar</t>
+  </si>
+  <si>
+    <t>Detalle</t>
+  </si>
+  <si>
+    <t>Pr. Unidad</t>
+  </si>
+  <si>
+    <t>Cantidad</t>
+  </si>
+  <si>
+    <t>Total</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   </t>
+  </si>
+  <si>
+    <t>{{item.ProductName}}</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> {{item.Quantity}}</t>
+  </si>
+  <si>
+    <t>{{item.TotalCost}}</t>
+  </si>
+  <si>
+    <t>{{TotalProducts}}</t>
+  </si>
+  <si>
+    <t>FACTURA #{{InvoiceNumber}}</t>
+  </si>
+  <si>
+    <t>{{InvoiceDate}}</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> {{item.Price}}</t>
   </si>
 </sst>
 </file>
@@ -153,7 +164,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="11">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -174,8 +185,49 @@
       <left/>
       <right/>
       <top/>
+      <bottom style="thick">
+        <color rgb="FF0070C0"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
       <bottom style="thin">
-        <color rgb="FF0070C0"/>
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
       </bottom>
       <diagonal/>
     </border>
@@ -183,7 +235,7 @@
       <left/>
       <right/>
       <top style="thin">
-        <color rgb="FF0070C0"/>
+        <color indexed="64"/>
       </top>
       <bottom/>
       <diagonal/>
@@ -191,71 +243,11 @@
     <border>
       <left/>
       <right/>
-      <top/>
-      <bottom style="thick">
-        <color rgb="FF0070C0"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color rgb="FF0070C0"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF0070C0"/>
-      </left>
-      <right/>
       <top style="thin">
-        <color rgb="FF0070C0"/>
+        <color indexed="64"/>
       </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color rgb="FF0070C0"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF0070C0"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF0070C0"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF0070C0"/>
-      </left>
-      <right/>
-      <top/>
       <bottom style="thin">
-        <color rgb="FF0070C0"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color rgb="FF0070C0"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color rgb="FF0070C0"/>
+        <color indexed="64"/>
       </bottom>
       <diagonal/>
     </border>
@@ -263,9 +255,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyProtection="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1">
@@ -282,6 +274,32 @@
       <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
       <protection locked="0"/>
@@ -290,14 +308,16 @@
       <alignment horizontal="center" vertical="center" textRotation="90"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
@@ -322,39 +342,23 @@
       <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
       <protection locked="0"/>
     </xf>
   </cellXfs>
@@ -422,8 +426,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="4600575" y="304801"/>
-          <a:ext cx="2381250" cy="1279922"/>
+          <a:off x="4403178" y="301845"/>
+          <a:ext cx="2379936" cy="1276966"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -754,8 +758,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BB634801-5C5D-41C3-B0E6-CCA3FC1E49A2}">
   <dimension ref="A1:S19"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="60" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="Q23" sqref="Q23"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="145" zoomScaleNormal="145" zoomScaleSheetLayoutView="145" workbookViewId="0">
+      <selection activeCell="H16" sqref="H16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -788,179 +792,181 @@
       <c r="L1" s="1"/>
     </row>
     <row r="2" spans="1:19" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="15"/>
-      <c r="C2" s="15"/>
-      <c r="D2" s="15"/>
-      <c r="E2" s="15"/>
-      <c r="F2" s="15"/>
-      <c r="L2" s="6" t="s">
-        <v>16</v>
+      <c r="B2" s="23"/>
+      <c r="C2" s="23"/>
+      <c r="D2" s="23"/>
+      <c r="E2" s="23"/>
+      <c r="F2" s="23"/>
+      <c r="L2" s="13" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B3" s="10" t="s">
-        <v>6</v>
-      </c>
-      <c r="C3" s="11"/>
-      <c r="D3" s="11"/>
-      <c r="E3" s="11"/>
-      <c r="F3" s="11"/>
-      <c r="L3" s="7"/>
+      <c r="B3" s="18" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" s="19"/>
+      <c r="D3" s="19"/>
+      <c r="E3" s="19"/>
+      <c r="F3" s="19"/>
+      <c r="L3" s="14"/>
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B4" s="11"/>
-      <c r="C4" s="11"/>
-      <c r="D4" s="11"/>
-      <c r="E4" s="11"/>
-      <c r="F4" s="11"/>
-      <c r="L4" s="7"/>
+      <c r="B4" s="19"/>
+      <c r="C4" s="19"/>
+      <c r="D4" s="19"/>
+      <c r="E4" s="19"/>
+      <c r="F4" s="19"/>
+      <c r="L4" s="14"/>
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B5" s="11"/>
-      <c r="C5" s="11"/>
-      <c r="D5" s="11"/>
-      <c r="E5" s="11"/>
-      <c r="F5" s="11"/>
-      <c r="L5" s="7"/>
+      <c r="B5" s="19"/>
+      <c r="C5" s="19"/>
+      <c r="D5" s="19"/>
+      <c r="E5" s="19"/>
+      <c r="F5" s="19"/>
+      <c r="L5" s="14"/>
     </row>
     <row r="6" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="L6" s="7"/>
+      <c r="L6" s="14"/>
     </row>
     <row r="7" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B7" s="12" t="s">
-        <v>12</v>
-      </c>
-      <c r="C7" s="9"/>
-      <c r="D7" s="9"/>
-      <c r="E7" s="9"/>
-      <c r="F7" s="9"/>
-      <c r="L7" s="7"/>
+      <c r="B7" s="20" t="s">
+        <v>18</v>
+      </c>
+      <c r="C7" s="16"/>
+      <c r="D7" s="16"/>
+      <c r="E7" s="16"/>
+      <c r="F7" s="16"/>
+      <c r="L7" s="14"/>
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B8" s="9"/>
-      <c r="C8" s="9"/>
-      <c r="D8" s="9"/>
-      <c r="E8" s="9"/>
-      <c r="F8" s="9"/>
-      <c r="H8" s="14"/>
-      <c r="I8" s="14"/>
-      <c r="J8" s="14"/>
-      <c r="K8" s="14"/>
-      <c r="L8" s="7"/>
+      <c r="B8" s="16"/>
+      <c r="C8" s="16"/>
+      <c r="D8" s="16"/>
+      <c r="E8" s="16"/>
+      <c r="F8" s="16"/>
+      <c r="H8" s="22"/>
+      <c r="I8" s="22"/>
+      <c r="J8" s="22"/>
+      <c r="K8" s="22"/>
+      <c r="L8" s="14"/>
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B9" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="C9" s="13" t="s">
-        <v>9</v>
-      </c>
-      <c r="D9" s="13"/>
-      <c r="E9" s="13"/>
-      <c r="F9" s="13"/>
-      <c r="H9" s="16" t="s">
-        <v>13</v>
-      </c>
-      <c r="I9" s="17"/>
-      <c r="J9" s="17"/>
-      <c r="K9" s="18"/>
-      <c r="L9" s="7"/>
+      <c r="C9" s="21" t="s">
+        <v>5</v>
+      </c>
+      <c r="D9" s="21"/>
+      <c r="E9" s="21"/>
+      <c r="F9" s="21"/>
+      <c r="H9" s="6"/>
+      <c r="I9" s="6"/>
+      <c r="J9" s="6"/>
+      <c r="K9" s="6"/>
+      <c r="L9" s="14"/>
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B10" s="4"/>
-      <c r="H10" s="19"/>
-      <c r="I10" s="11"/>
-      <c r="J10" s="11"/>
-      <c r="K10" s="20"/>
-      <c r="L10" s="7"/>
+      <c r="E10" s="9"/>
+      <c r="H10" s="25"/>
+      <c r="I10" s="25"/>
+      <c r="J10" s="25"/>
+      <c r="K10" s="25"/>
+      <c r="L10" s="14"/>
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B11" s="4" t="s">
         <v>1</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="E11" s="4" t="s">
         <v>2</v>
       </c>
       <c r="F11" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="H11" s="19"/>
-      <c r="I11" s="11"/>
-      <c r="J11" s="11"/>
-      <c r="K11" s="20"/>
-      <c r="L11" s="7"/>
+        <v>19</v>
+      </c>
+      <c r="H11" s="24"/>
+      <c r="I11" s="24"/>
+      <c r="J11" s="24"/>
+      <c r="K11" s="24"/>
+      <c r="L11" s="14"/>
       <c r="P11"/>
       <c r="Q11"/>
       <c r="R11"/>
       <c r="S11"/>
     </row>
     <row r="12" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="H12" s="21"/>
-      <c r="I12" s="22"/>
-      <c r="J12" s="22"/>
-      <c r="K12" s="23"/>
-      <c r="L12" s="7"/>
+      <c r="H12" s="16" t="s">
+        <v>3</v>
+      </c>
+      <c r="I12" s="16"/>
+      <c r="J12" s="16"/>
+      <c r="K12" s="16"/>
+      <c r="L12" s="14"/>
       <c r="P12"/>
       <c r="Q12"/>
       <c r="R12"/>
       <c r="S12"/>
     </row>
     <row r="13" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B13" s="14" t="s">
-        <v>3</v>
-      </c>
-      <c r="C13" s="14"/>
-      <c r="D13" s="14"/>
-      <c r="E13" s="14" t="s">
-        <v>4</v>
-      </c>
-      <c r="F13" s="14"/>
-      <c r="H13" s="24"/>
-      <c r="I13" s="24"/>
-      <c r="J13" s="24"/>
-      <c r="K13" s="24"/>
-      <c r="L13" s="7"/>
+      <c r="B13" s="26" t="s">
+        <v>9</v>
+      </c>
+      <c r="C13" s="27"/>
+      <c r="D13" s="28"/>
+      <c r="E13" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="F13" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="G13" s="11"/>
+      <c r="H13" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="L13" s="14"/>
       <c r="P13"/>
       <c r="Q13"/>
       <c r="R13"/>
       <c r="S13"/>
     </row>
     <row r="14" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B14" s="8" t="s">
+      <c r="B14" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="C14" s="8"/>
-      <c r="D14" s="8"/>
-      <c r="E14" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="F14" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="H14" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="I14" s="9"/>
-      <c r="J14" s="9"/>
-      <c r="K14" s="9"/>
-      <c r="L14" s="7"/>
+      <c r="C14" s="15"/>
+      <c r="D14" s="15"/>
+      <c r="E14" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="F14" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="G14" s="11"/>
+      <c r="H14" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="L14" s="14"/>
       <c r="P14"/>
       <c r="Q14"/>
       <c r="R14"/>
       <c r="S14"/>
     </row>
     <row r="15" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B15" s="8"/>
-      <c r="C15" s="8"/>
-      <c r="D15" s="8"/>
-      <c r="H15" s="3"/>
+      <c r="B15" s="17"/>
+      <c r="C15" s="17"/>
+      <c r="D15" s="17"/>
+      <c r="F15" s="12"/>
+      <c r="G15" s="12"/>
       <c r="I15" s="3"/>
       <c r="J15" s="3"/>
       <c r="K15" s="3"/>
-      <c r="L15" s="7"/>
+      <c r="L15" s="14"/>
       <c r="P15"/>
       <c r="Q15"/>
       <c r="R15"/>
@@ -971,14 +977,18 @@
       <c r="B16"/>
       <c r="C16"/>
       <c r="D16"/>
-      <c r="E16"/>
+      <c r="E16" s="2" t="s">
+        <v>13</v>
+      </c>
       <c r="F16"/>
       <c r="G16"/>
-      <c r="H16"/>
+      <c r="H16" s="8" t="s">
+        <v>17</v>
+      </c>
       <c r="I16"/>
       <c r="J16"/>
       <c r="K16"/>
-      <c r="L16" s="7"/>
+      <c r="L16" s="14"/>
       <c r="P16"/>
       <c r="Q16"/>
       <c r="R16"/>
@@ -986,25 +996,27 @@
     </row>
     <row r="19" spans="16:16" x14ac:dyDescent="0.25">
       <c r="P19" s="2" t="s">
-        <v>15</v>
+        <v>7</v>
       </c>
     </row>
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" selectLockedCells="1"/>
-  <mergeCells count="13">
+  <mergeCells count="15">
+    <mergeCell ref="F13:G13"/>
+    <mergeCell ref="F14:G14"/>
+    <mergeCell ref="F15:G15"/>
     <mergeCell ref="L2:L16"/>
     <mergeCell ref="B14:D14"/>
-    <mergeCell ref="H14:K14"/>
+    <mergeCell ref="H12:K12"/>
     <mergeCell ref="B15:D15"/>
     <mergeCell ref="B3:F5"/>
     <mergeCell ref="B7:F8"/>
     <mergeCell ref="C9:F9"/>
     <mergeCell ref="H8:K8"/>
     <mergeCell ref="B2:F2"/>
+    <mergeCell ref="H11:K11"/>
+    <mergeCell ref="H10:K10"/>
     <mergeCell ref="B13:D13"/>
-    <mergeCell ref="E13:F13"/>
-    <mergeCell ref="H9:K12"/>
-    <mergeCell ref="H13:K13"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="77" orientation="portrait" r:id="rId1"/>

</xml_diff>